<commit_message>
Final Changes 31 Dec
</commit_message>
<xml_diff>
--- a/src/main/java/testData/SignUpData.xlsx
+++ b/src/main/java/testData/SignUpData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
-  <si>
-    <t>excelTest</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>FirstAnswer</t>
   </si>
@@ -127,6 +125,15 @@
   </si>
   <si>
     <t>Tom Company One</t>
+  </si>
+  <si>
+    <t>testSignUpFirstPage</t>
+  </si>
+  <si>
+    <t>testLoginPage</t>
+  </si>
+  <si>
+    <t>apandhe5@xpanxion.com</t>
   </si>
 </sst>
 </file>
@@ -459,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,105 +497,105 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E2" s="2">
         <v>4564654560</v>
       </c>
       <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L2" s="2">
         <v>456</v>
@@ -597,22 +604,22 @@
         <v>4564564560</v>
       </c>
       <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>29</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>30</v>
       </c>
       <c r="R2" s="2">
         <v>10001</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T2" s="2">
         <v>1111</v>
@@ -631,4 +638,49 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>